<commit_message>
Updated POD_Excluded.xlsx from OneDrive
</commit_message>
<xml_diff>
--- a/POD_Excluded.xlsx
+++ b/POD_Excluded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarek Mahran\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CADE55-E152-4BA2-90F7-C8B233BA1CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3F7B65-2D12-43A3-B469-1B4D7F8C56C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{5B47CC1A-8461-4682-B8BC-6BD2DADA04DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="267">
   <si>
     <t>Status</t>
   </si>
@@ -228,6 +228,615 @@
   </si>
   <si>
     <t>WO-2025101239895570</t>
+  </si>
+  <si>
+    <t>CM20251001000806</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00001393</t>
+  </si>
+  <si>
+    <t>TT-20251001-01378</t>
+  </si>
+  <si>
+    <t>SRIY0042</t>
+  </si>
+  <si>
+    <t>CM20251002000991</t>
+  </si>
+  <si>
+    <t>PCM-20251002-00001553</t>
+  </si>
+  <si>
+    <t>TT-20250903-01304</t>
+  </si>
+  <si>
+    <t>SRIY0073</t>
+  </si>
+  <si>
+    <t>CM20251002000992</t>
+  </si>
+  <si>
+    <t>PCM-20251002-00001554</t>
+  </si>
+  <si>
+    <t>CM20251004000081</t>
+  </si>
+  <si>
+    <t>PCM-20251004-00000159</t>
+  </si>
+  <si>
+    <t>TT-20251004-00191</t>
+  </si>
+  <si>
+    <t>RIY0643</t>
+  </si>
+  <si>
+    <t>CM20251004001174</t>
+  </si>
+  <si>
+    <t>PCM-20251004-00001893</t>
+  </si>
+  <si>
+    <t>TT-20251004-01908</t>
+  </si>
+  <si>
+    <t>RIY0496</t>
+  </si>
+  <si>
+    <t>CM20251004001176</t>
+  </si>
+  <si>
+    <t>PCM-20251004-00001895</t>
+  </si>
+  <si>
+    <t>TT-20251004-01911</t>
+  </si>
+  <si>
+    <t>CM20251004001177</t>
+  </si>
+  <si>
+    <t>PCM-20251004-00001896</t>
+  </si>
+  <si>
+    <t>TT-20251004-01912</t>
+  </si>
+  <si>
+    <t>CM20251006000267</t>
+  </si>
+  <si>
+    <t>PCM-20251006-00000517</t>
+  </si>
+  <si>
+    <t>TT-20251006-00705</t>
+  </si>
+  <si>
+    <t>MDN0325</t>
+  </si>
+  <si>
+    <t>CM20251003000918</t>
+  </si>
+  <si>
+    <t>PCM-20251003-00001529</t>
+  </si>
+  <si>
+    <t>TT-20251003-01528</t>
+  </si>
+  <si>
+    <t>HLHD0710</t>
+  </si>
+  <si>
+    <t>CM20251003000917</t>
+  </si>
+  <si>
+    <t>PCM-20251003-00001527</t>
+  </si>
+  <si>
+    <t>TT-20251003-01542</t>
+  </si>
+  <si>
+    <t>HLHD0709</t>
+  </si>
+  <si>
+    <t>CM20251004001281</t>
+  </si>
+  <si>
+    <t>PCM-20251004-00002090</t>
+  </si>
+  <si>
+    <t>CM20251008000857</t>
+  </si>
+  <si>
+    <t>PCM-20251008-00001662</t>
+  </si>
+  <si>
+    <t>TT-20251008-01710</t>
+  </si>
+  <si>
+    <t>MDYB2549</t>
+  </si>
+  <si>
+    <t>CM20251001000116</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00000214</t>
+  </si>
+  <si>
+    <t>TT-20250930-02028</t>
+  </si>
+  <si>
+    <t>Region_1</t>
+  </si>
+  <si>
+    <t>SAR0074</t>
+  </si>
+  <si>
+    <t>CM20251001000130</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00000234</t>
+  </si>
+  <si>
+    <t>TT-20250930-02215</t>
+  </si>
+  <si>
+    <t>SAR0076</t>
+  </si>
+  <si>
+    <t>CM20251001000644</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00001167</t>
+  </si>
+  <si>
+    <t>TT-20251001-01074</t>
+  </si>
+  <si>
+    <t>DAM0270</t>
+  </si>
+  <si>
+    <t>CM20251001000926</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00001554</t>
+  </si>
+  <si>
+    <t>TT-20251001-01483</t>
+  </si>
+  <si>
+    <t>SHMBY0039</t>
+  </si>
+  <si>
+    <t>CM20251001000964</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00001620</t>
+  </si>
+  <si>
+    <t>TT-20251001-01556</t>
+  </si>
+  <si>
+    <t>SHMBY0043</t>
+  </si>
+  <si>
+    <t>CM20251001000989</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00001653</t>
+  </si>
+  <si>
+    <t>TT-20251001-01573</t>
+  </si>
+  <si>
+    <t>SHMBY0044</t>
+  </si>
+  <si>
+    <t>CM20251001001138</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00001885</t>
+  </si>
+  <si>
+    <t>TT-20251001-01798</t>
+  </si>
+  <si>
+    <t>SHMBY0040</t>
+  </si>
+  <si>
+    <t>CM20251001001272</t>
+  </si>
+  <si>
+    <t>PCM-20251001-00002103</t>
+  </si>
+  <si>
+    <t>TT-20251001-01863</t>
+  </si>
+  <si>
+    <t>KBR0171</t>
+  </si>
+  <si>
+    <t>CM20251002001538</t>
+  </si>
+  <si>
+    <t>PCM-20251002-00002387</t>
+  </si>
+  <si>
+    <t>TT-20251002-02666</t>
+  </si>
+  <si>
+    <t>DMHF0079</t>
+  </si>
+  <si>
+    <t>CM20251005000398</t>
+  </si>
+  <si>
+    <t>PCM-20251005-00001186</t>
+  </si>
+  <si>
+    <t>TT-20251005-01319</t>
+  </si>
+  <si>
+    <t>KBR6093</t>
+  </si>
+  <si>
+    <t>CM20251005000601</t>
+  </si>
+  <si>
+    <t>PCM-20251005-00001520</t>
+  </si>
+  <si>
+    <t>TT-20251005-01309</t>
+  </si>
+  <si>
+    <t>DAM2729</t>
+  </si>
+  <si>
+    <t>CM20251006000176</t>
+  </si>
+  <si>
+    <t>PCM-20251006-00000361</t>
+  </si>
+  <si>
+    <t>TT-20251006-00549</t>
+  </si>
+  <si>
+    <t>DAM0389</t>
+  </si>
+  <si>
+    <t>CM20251006000247</t>
+  </si>
+  <si>
+    <t>PCM-20251006-00000487</t>
+  </si>
+  <si>
+    <t>TT-20251006-00677</t>
+  </si>
+  <si>
+    <t>DAM2820</t>
+  </si>
+  <si>
+    <t>CM20251006000318</t>
+  </si>
+  <si>
+    <t>PCM-20251006-00000604</t>
+  </si>
+  <si>
+    <t>TT-20251006-00800</t>
+  </si>
+  <si>
+    <t>JB1</t>
+  </si>
+  <si>
+    <t>CM20251006001308</t>
+  </si>
+  <si>
+    <t>PCM-20251006-00002228</t>
+  </si>
+  <si>
+    <t>TT-20251006-02316</t>
+  </si>
+  <si>
+    <t>DAM2802</t>
+  </si>
+  <si>
+    <t>CM20251007000074</t>
+  </si>
+  <si>
+    <t>PCM-20251007-00000145</t>
+  </si>
+  <si>
+    <t>TT-20251007-00162</t>
+  </si>
+  <si>
+    <t>RAF0095</t>
+  </si>
+  <si>
+    <t>CM20251007001218</t>
+  </si>
+  <si>
+    <t>PCM-20251007-00002085</t>
+  </si>
+  <si>
+    <t>TT-20251007-01644</t>
+  </si>
+  <si>
+    <t>KBR2788</t>
+  </si>
+  <si>
+    <t>CM20251007001335</t>
+  </si>
+  <si>
+    <t>PCM-20251007-00002292</t>
+  </si>
+  <si>
+    <t>TT-20251007-02050</t>
+  </si>
+  <si>
+    <t>TRT2996</t>
+  </si>
+  <si>
+    <t>CM20251010000047</t>
+  </si>
+  <si>
+    <t>PCM-20251010-00000111</t>
+  </si>
+  <si>
+    <t>TT-20251010-00105</t>
+  </si>
+  <si>
+    <t>RYDM0075</t>
+  </si>
+  <si>
+    <t>CM20251010000168</t>
+  </si>
+  <si>
+    <t>PCM-20251010-00000325</t>
+  </si>
+  <si>
+    <t>TT-20251010-00393</t>
+  </si>
+  <si>
+    <t>ARR0518</t>
+  </si>
+  <si>
+    <t>CM20251011000088</t>
+  </si>
+  <si>
+    <t>PCM-20251011-00000180</t>
+  </si>
+  <si>
+    <t>TT-20251011-00188</t>
+  </si>
+  <si>
+    <t>QRY2605</t>
+  </si>
+  <si>
+    <t>CM20251012001555</t>
+  </si>
+  <si>
+    <t>PCM-20251012-00002447</t>
+  </si>
+  <si>
+    <t>TT-20251012-02529</t>
+  </si>
+  <si>
+    <t>JBL2927</t>
+  </si>
+  <si>
+    <t>CM20251013000003</t>
+  </si>
+  <si>
+    <t>PCM-20251013-00000008</t>
+  </si>
+  <si>
+    <t>TT-20251013-00005</t>
+  </si>
+  <si>
+    <t>ARM2759</t>
+  </si>
+  <si>
+    <t>2025-10-01 14:56:59</t>
+  </si>
+  <si>
+    <t>2025-10-02 15:36:12</t>
+  </si>
+  <si>
+    <t>2025-10-02 15:36:45</t>
+  </si>
+  <si>
+    <t>2025-10-04 03:24:24</t>
+  </si>
+  <si>
+    <t>2025-10-04 21:06:57</t>
+  </si>
+  <si>
+    <t>2025-10-04 21:09:02</t>
+  </si>
+  <si>
+    <t>2025-10-04 21:09:33</t>
+  </si>
+  <si>
+    <t>2025-10-06 07:05:31</t>
+  </si>
+  <si>
+    <t>2025-10-03 20:30:47</t>
+  </si>
+  <si>
+    <t>2025-10-03 20:30:27</t>
+  </si>
+  <si>
+    <t>2025-10-04 23:48:35</t>
+  </si>
+  <si>
+    <t>2025-10-08 15:21:14</t>
+  </si>
+  <si>
+    <t>2025-10-01 02:31:32</t>
+  </si>
+  <si>
+    <t>2025-10-01 02:49:43</t>
+  </si>
+  <si>
+    <t>2025-10-01 12:31:51</t>
+  </si>
+  <si>
+    <t>2025-10-01 15:53:57</t>
+  </si>
+  <si>
+    <t>2025-10-01 16:31:15</t>
+  </si>
+  <si>
+    <t>2025-10-01 16:50:10</t>
+  </si>
+  <si>
+    <t>2025-10-01 18:38:03</t>
+  </si>
+  <si>
+    <t>2025-10-01 21:30:27</t>
+  </si>
+  <si>
+    <t>2025-10-02 23:56:01</t>
+  </si>
+  <si>
+    <t>2025-10-05 06:58:29</t>
+  </si>
+  <si>
+    <t>2025-10-05 10:01:56</t>
+  </si>
+  <si>
+    <t>2025-10-06 04:50:08</t>
+  </si>
+  <si>
+    <t>2025-10-06 06:44:53</t>
+  </si>
+  <si>
+    <t>2025-10-06 08:10:34</t>
+  </si>
+  <si>
+    <t>2025-10-06 22:31:53</t>
+  </si>
+  <si>
+    <t>2025-10-07 01:48:57</t>
+  </si>
+  <si>
+    <t>2025-10-07 19:08:59</t>
+  </si>
+  <si>
+    <t>2025-10-07 21:14:01</t>
+  </si>
+  <si>
+    <t>2025-10-10 01:38:31</t>
+  </si>
+  <si>
+    <t>2025-10-10 06:55:50</t>
+  </si>
+  <si>
+    <t>2025-10-11 02:38:51</t>
+  </si>
+  <si>
+    <t>2025-10-12 22:47:53</t>
+  </si>
+  <si>
+    <t>2025-10-13 00:10:32</t>
+  </si>
+  <si>
+    <t>ETH_LOS at SRIY0042/SRIY0043_NE_1 @ Sceco</t>
+  </si>
+  <si>
+    <t>ETH_LOS at SRIY0073/SRIY0074_NE_1 @ Sceco</t>
+  </si>
+  <si>
+    <t>ETH_LOS at RIY0643_NE_24_H @ Sceco</t>
+  </si>
+  <si>
+    <t>RF Unit Maintenance Link Failure at RIY0496-P2_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>BBU CPRI Optical Module Fault at RIY0496-P2_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>NR Cell Unavailable at RIY0496-P2_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>GSM Local Cell Capability Decline at MDN2M1325-P1-HRM @ Sceco</t>
+  </si>
+  <si>
+    <t>External Clock Reference Problem at HLHD2M5710-P3 @ Generator_SG</t>
+  </si>
+  <si>
+    <t>External Clock Reference Problem at HLHD2M5709-P3 @ Generator_SG</t>
+  </si>
+  <si>
+    <t>MW RTN Observing MW_BER_SD,MW_BER_SD,MW_BER_SD,MW_BER_SD,MW_BER_SD at MDYB2549_NE_1</t>
+  </si>
+  <si>
+    <t>2(2G) 2(3G) 2(LTE) sites down under SAR0073-P1-HUB-USF,SAR0074-P1-HUB-USF/SK1BSCH01 @ Generator_DG</t>
+  </si>
+  <si>
+    <t>2(2G) 2(3G) 2(LTE) sites down under SAR0076-P1-HUB-USF,SAR0075-P1-DIA-HUB-USF/SK1BSCH01 @ Generator_DG</t>
+  </si>
+  <si>
+    <t>Cell RX Channel Interference Noise Power Unbalanced at DAM2M7270-P1-SHOP-HUB-WDM-L800 @ Sceco</t>
+  </si>
+  <si>
+    <t>GPS Locked Satellites Insufficient at SHMBY0039-P3_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>GPS Locked Satellites Insufficient at SHMBY0043-P3_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>GPS Locked Satellites Insufficient at SHMBY0044-P3_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>GPS Locked Satellites Insufficient at SHMBY0040-P3_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>GNSS Locked Satellites Insufficient at KBR0171-P3_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>1(2G) sites down under DMHF0079-P3/R1_HF_HWBSC01 @ Generator_SG</t>
+  </si>
+  <si>
+    <t>RFC Port Underpower at KBR6093-DCU1 @ Sceco</t>
+  </si>
+  <si>
+    <t>GNSS Clock Output Unavailable at DAM2729-P2_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>OSC_LOS at DAM0389_HYB @ Sceco</t>
+  </si>
+  <si>
+    <t>GNSS Locked Satellites Insufficient at DAM2820-P3_SRAN @ Generator_SG</t>
+  </si>
+  <si>
+    <t>LINK DOWN  at JB1-ASG-01 TT-20250915-00318 @ Sceco_STB</t>
+  </si>
+  <si>
+    <t>Cell RX Channel Interference Noise Power Unbalanced at DAM2M8802-CA-L800-FWA-P1-VIP @ Sceco</t>
+  </si>
+  <si>
+    <t>RF Unit TX Channel Gain Out of Range at RAF0095-P2_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>1(5G) sites down under KBR2788-P3_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>2(2G) 1(3G) 2(LTE) sites down under TRT2996-P2,TRT0764-P3/R1_DM_HWBSC01 @ Sceco</t>
+  </si>
+  <si>
+    <t>1(LTE) sites down under RYDM0075-L800-P3 @ Sceco_STB</t>
+  </si>
+  <si>
+    <t>Overlow Input Power of Optical Module at Arar-0518-NE40E-X8-PE-01 @ Sceco_STB</t>
+  </si>
+  <si>
+    <t>RF Unit RX Channel RTWP/RSSI Unbalanced at QRY2605-P3-USF_SRAN @ Sceco</t>
+  </si>
+  <si>
+    <t>BUS_ERR at JBL2927_NE_1_SDB @ Sceco</t>
+  </si>
+  <si>
+    <t>1(LTE) sites down under ARM2759-P1_SRAN-PC @ Power Cube</t>
   </si>
 </sst>
 </file>
@@ -235,7 +844,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -343,50 +952,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -414,6 +991,38 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -764,10 +1373,10 @@
     <tableColumn id="4" xr3:uid="{2C08E557-46C7-4559-9F2E-6A6AB3C7BD19}" name="TT ID" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{EBECD3F7-8AC2-435F-BC0C-7BBF5969F615}" name="TT Type" dataDxfId="5"/>
     <tableColumn id="6" xr3:uid="{B8FCEE44-2024-47E9-83A0-AB44E7A091C4}" name="Region" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{F8012F2B-4C01-429A-8216-2A8B6A726AA4}" name="Site ID" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{D8A842A2-5725-4D78-BA01-41E074F2D808}" name="Site Name" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{54F2B62D-9BB3-49EE-9679-CCC8172888ED}" name="Created At" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{E55C36AA-3E83-4908-8794-22DCAC60C77A}" name="Title" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{F8012F2B-4C01-429A-8216-2A8B6A726AA4}" name="Site ID" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{D8A842A2-5725-4D78-BA01-41E074F2D808}" name="Site Name" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{54F2B62D-9BB3-49EE-9679-CCC8172888ED}" name="Created At" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{E55C36AA-3E83-4908-8794-22DCAC60C77A}" name="Title" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1090,7 +1699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2991AF72-FEEC-4E39-9F69-CFE706A3AA5B}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -1106,7 +1715,7 @@
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1701,6 +2310,916 @@
       </c>
       <c r="J21" s="6" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="J49" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="J56" s="6" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>